<commit_message>
fixed kalgor advancements to apply from prev advancements to future weaons
</commit_message>
<xml_diff>
--- a/units/Kalgor_Advancements.xlsx
+++ b/units/Kalgor_Advancements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c009ef319659ad0f/Dokumente/My Games/Wesnoth1.16/data/add-ons/Deception/units/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c009ef319659ad0f/Dokumente/My Games/Wesnoth1.16/data/add-ons/deception/units/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="167" documentId="11_F25DC773A252ABDACC1048AA191E4DF65BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3928EB9E-9261-48EE-A3EC-64034E33B01B}"/>
+  <xr:revisionPtr revIDLastSave="201" documentId="11_F25DC773A252ABDACC1048AA191E4DF65BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A474F050-0BA5-4B7B-907A-BD3E7F113775}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="12186" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Advancement</t>
   </si>
@@ -83,16 +83,10 @@
     <t>strength3</t>
   </si>
   <si>
-    <t>abyss1</t>
-  </si>
-  <si>
-    <t>abyss2</t>
-  </si>
-  <si>
-    <t>darkness1</t>
-  </si>
-  <si>
-    <t>darkness2</t>
+    <t>abyss</t>
+  </si>
+  <si>
+    <t>darkness</t>
   </si>
 </sst>
 </file>
@@ -139,10 +133,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -439,31 +433,31 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.5">
       <c r="B2" s="1" t="s">
@@ -560,7 +554,7 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D22" si="0">B4*C4</f>
+        <f t="shared" ref="D4:D20" si="0">B4*C4</f>
         <v>30</v>
       </c>
       <c r="E4">
@@ -570,73 +564,73 @@
         <v>4</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G22" si="1">E4*F4</f>
+        <f t="shared" ref="G4:G20" si="1">E4*F4</f>
         <v>32</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J22" si="2">H4*I4</f>
+        <f t="shared" ref="J4:J20" si="2">H4*I4</f>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M22" si="3">K4*L4</f>
+        <f t="shared" ref="M4:M20" si="3">K4*L4</f>
         <v>0</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P22" si="4">N4*O4</f>
+        <f t="shared" ref="P4:P20" si="4">N4*O4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>19</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>2</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>10</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>4</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>13</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>3</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>10</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>2</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="2">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>5</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="2">
         <v>3</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="2">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
@@ -666,22 +660,34 @@
         <v>44</v>
       </c>
       <c r="H6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I6">
         <v>3</v>
       </c>
       <c r="J6">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="K6">
+        <v>11</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
       </c>
       <c r="M6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="N6">
+        <v>7</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
       </c>
       <c r="P6">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.5">
@@ -709,22 +715,34 @@
         <v>48</v>
       </c>
       <c r="H7">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I7">
         <v>3</v>
       </c>
       <c r="J7">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="K7">
+        <v>12</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
       </c>
       <c r="M7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="N7">
+        <v>9</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
       </c>
       <c r="P7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.5">
@@ -752,22 +770,34 @@
         <v>52</v>
       </c>
       <c r="H8">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I8">
         <v>3</v>
       </c>
       <c r="J8">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>57</v>
+      </c>
+      <c r="K8">
+        <v>13</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
       </c>
       <c r="M8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="N8">
+        <v>11</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
       </c>
       <c r="P8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.5">
@@ -787,14 +817,14 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L9">
         <v>3</v>
       </c>
       <c r="M9">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="P9">
         <f t="shared" si="4"/>
@@ -817,25 +847,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K10">
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N10">
         <v>12</v>
       </c>
-      <c r="L10">
-        <v>3</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="3"/>
-        <v>36</v>
+      <c r="O10">
+        <v>4</v>
       </c>
       <c r="P10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
       <c r="D11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -852,21 +879,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N11">
-        <v>9</v>
-      </c>
-      <c r="O11">
-        <v>3</v>
-      </c>
       <c r="P11">
         <f t="shared" si="4"/>
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
       <c r="D12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -883,15 +901,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N12">
-        <v>12</v>
-      </c>
-      <c r="O12">
-        <v>3</v>
-      </c>
       <c r="P12">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.5">
@@ -1066,50 +1078,6 @@
         <v>0</v>
       </c>
       <c r="P20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.5">
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="4:16" x14ac:dyDescent="0.5">
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>

</xml_diff>